<commit_message>
update readme and complete the feedback
</commit_message>
<xml_diff>
--- a/feedback/log.xlsx
+++ b/feedback/log.xlsx
@@ -158,12 +158,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,37 +173,92 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -215,15 +270,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,93 +287,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,61 +325,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,19 +481,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,97 +505,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,15 +516,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -546,6 +530,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,17 +558,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,15 +593,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -623,153 +601,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1128,7 +1121,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1212,7 +1205,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1239,6 +1232,12 @@
       </c>
       <c r="I5">
         <v>58333344</v>
+      </c>
+      <c r="J5">
+        <v>3141592</v>
+      </c>
+      <c r="K5">
+        <v>2718281</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1276,7 +1275,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1303,6 +1302,12 @@
       </c>
       <c r="I7">
         <v>733846</v>
+      </c>
+      <c r="J7">
+        <v>54321</v>
+      </c>
+      <c r="K7">
+        <v>123456</v>
       </c>
     </row>
     <row r="8" spans="1:11">

</xml_diff>

<commit_message>
add general mode to generatedata for testing
</commit_message>
<xml_diff>
--- a/feedback/log.xlsx
+++ b/feedback/log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>读入时间</t>
   </si>
@@ -151,6 +151,27 @@
   </si>
   <si>
     <t xml:space="preserve"> 1034ms</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>2341ms</t>
+  </si>
+  <si>
+    <t>10ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2ms</t>
+  </si>
+  <si>
+    <t>58ms</t>
+  </si>
+  <si>
+    <t>78ms</t>
+  </si>
+  <si>
+    <t>64ms</t>
   </si>
 </sst>
 </file>
@@ -158,8 +179,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -173,66 +194,66 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,6 +267,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -255,7 +284,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -263,54 +307,31 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,13 +346,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,163 +442,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,6 +537,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -530,15 +560,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,8 +581,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -593,11 +616,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,10 +645,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -636,133 +657,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1118,10 +1139,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1378,6 +1399,41 @@
       </c>
       <c r="K9">
         <v>2000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10">
+        <v>20000</v>
+      </c>
+      <c r="I10">
+        <v>100000</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>